<commit_message>
rearrange folder of static
</commit_message>
<xml_diff>
--- a/docs/Tasks Arrangement.xlsx
+++ b/docs/Tasks Arrangement.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>项目任务安排表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +55,22 @@
   </si>
   <si>
     <t>/index/inex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015年10月26日14:42:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预计完成日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015年10月26日14:43:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -101,9 +117,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -405,107 +424,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
+    <col min="1" max="1" width="14.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.25" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="12.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.25" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1">
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
         <v>10</v>
       </c>
     </row>

</xml_diff>